<commit_message>
Freeze 2nd row of the excel sheets so headers will be always on top
</commit_message>
<xml_diff>
--- a/assets/Template/ActionListTemplate.xlsx
+++ b/assets/Template/ActionListTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masaki.kumamoto\OneDrive - UiPath\Documents\UiPath\00_DemoMaster\DocumentUnderstanding\DU_IntelligentFormExtractorPocPack\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/masaki_kumamoto_uipath_com/Documents/Documents/UiPath/04_Templates/DocumentUnderstandingEvaluationTemplate/assets/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914C0D11-656D-4C91-9AAB-9E23FE0702BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{914C0D11-656D-4C91-9AAB-9E23FE0702BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F4769BF-1214-4A5E-95FC-0734E9D94DA4}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="1260" windowWidth="31320" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="-18225" windowWidth="35205" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="4" r:id="rId1"/>
@@ -410,7 +410,8 @@
   <dimension ref="B2:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>